<commit_message>
- fixed corrected age calculation algorithm - added option to switch from median- to mean-function for outlier-detection
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/Ratios.xlsx
+++ b/data/CPR_100221_20210210-114741/Ratios.xlsx
@@ -412,7 +412,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
@@ -497,10 +497,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2">
-        <v>0.1143667343042054</v>
+        <v>-1.385999438767938</v>
       </c>
       <c r="B2">
-        <v>0.001672089322806292</v>
+        <v>0.001669580863432305</v>
       </c>
       <c r="C2">
         <v>0.009947044687815326</v>
@@ -559,10 +559,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3">
-        <v>146.0150489192544</v>
+        <v>144.2958033305279</v>
       </c>
       <c r="B3">
-        <v>0.0005483835799002634</v>
+        <v>0.0005475608978145764</v>
       </c>
       <c r="C3">
         <v>0.009972045011614569</v>
@@ -621,10 +621,10 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4">
-        <v>0.07524374222045438</v>
+        <v>-1.425063738750176</v>
       </c>
       <c r="B4">
-        <v>0.001847658475256469</v>
+        <v>0.001844886627987924</v>
       </c>
       <c r="C4">
         <v>0.01002745745125579</v>
@@ -683,10 +683,10 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5">
-        <v>145.9566434423649</v>
+        <v>144.2374854732194</v>
       </c>
       <c r="B5">
-        <v>0.0004972629048417086</v>
+        <v>0.0004965169137167292</v>
       </c>
       <c r="C5">
         <v>0.01000467291249881</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6">
-        <v>2.514640426850789</v>
+        <v>1.010673376144799</v>
       </c>
       <c r="B6">
-        <v>0.001802158364614082</v>
+        <v>0.001799454776365855</v>
       </c>
       <c r="C6">
         <v>0.009819163185528878</v>
@@ -807,10 +807,10 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7">
-        <v>146.3587040911574</v>
+        <v>144.6389429527974</v>
       </c>
       <c r="B7">
-        <v>0.0005473663981895642</v>
+        <v>0.0005465452420743875</v>
       </c>
       <c r="C7">
         <v>0.009974392941727757</v>
@@ -869,10 +869,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8">
-        <v>0.6979624794027917</v>
+        <v>-0.8032792008549894</v>
       </c>
       <c r="B8">
-        <v>0.001333396989833812</v>
+        <v>0.001331396634869054</v>
       </c>
       <c r="C8">
         <v>0.009907802217358631</v>
@@ -931,10 +931,10 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9">
-        <v>145.9930428814786</v>
+        <v>144.2738303060913</v>
       </c>
       <c r="B9">
-        <v>0.0003793789222423742</v>
+        <v>0.0003788097800316013</v>
       </c>
       <c r="C9">
         <v>0.009984642247515869</v>
@@ -993,10 +993,10 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10">
-        <v>0.7046473595699876</v>
+        <v>-0.7966043493090602</v>
       </c>
       <c r="B10">
-        <v>0.001929450337261307</v>
+        <v>0.001926555786283</v>
       </c>
       <c r="C10">
         <v>0.009841760080815906</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11">
-        <v>146.9604677031626</v>
+        <v>145.2398038022811</v>
       </c>
       <c r="B11">
-        <v>0.0004881335238397607</v>
+        <v>0.0004874012285628684</v>
       </c>
       <c r="C11">
         <v>0.01001695123005385</v>
@@ -1117,10 +1117,10 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12">
-        <v>1.121018406509577</v>
+        <v>-0.3808579399658951</v>
       </c>
       <c r="B12">
-        <v>0.001506192629674534</v>
+        <v>0.00150393304762386</v>
       </c>
       <c r="C12">
         <v>0.009956225754944125</v>

</xml_diff>

<commit_message>
changes to error calculation changed to gui and excel formatting
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/Ratios.xlsx
+++ b/data/CPR_100221_20210210-114741/Ratios.xlsx
@@ -423,7 +423,7 @@
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
@@ -440,7 +440,7 @@
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
     <col min="18" max="18" width="20.7109375" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="23.7109375" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" customWidth="1"/>
     <col min="21" max="21" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,10 +514,10 @@
         <v>10815</v>
       </c>
       <c r="B2" s="1">
-        <v>-1.385999438767938</v>
+        <v>-1.576667569721746</v>
       </c>
       <c r="C2" s="1">
-        <v>0.001669580863432305</v>
+        <v>0.001478752354046088</v>
       </c>
       <c r="D2" s="1">
         <v>0.009947044687815326</v>
@@ -526,10 +526,10 @@
         <v>0.7011526860997377</v>
       </c>
       <c r="F2" s="1">
-        <v>0.00714433689233078</v>
+        <v>0.007144296897712548</v>
       </c>
       <c r="G2" s="1">
-        <v>0.007046489093913378</v>
+        <v>0.007417903189274322</v>
       </c>
       <c r="H2" s="1">
         <v>2.732204386789063</v>
@@ -538,28 +538,28 @@
         <v>0.01064431016615503</v>
       </c>
       <c r="J2" s="1">
-        <v>2.082960841733835</v>
+        <v>2.083253286508519</v>
       </c>
       <c r="K2" s="1">
-        <v>0.6365650677998222</v>
+        <v>0.6590415179803142</v>
       </c>
       <c r="L2" s="1">
-        <v>0.00756863612888841</v>
+        <v>0.007567191028275208</v>
       </c>
       <c r="M2" s="1">
-        <v>0.1671898113278986</v>
+        <v>0.1481087536733177</v>
       </c>
       <c r="N2" s="1">
-        <v>5.489252419759365E-05</v>
+        <v>5.488204341624448E-05</v>
       </c>
       <c r="O2" s="1">
-        <v>0.1671898113278987</v>
+        <v>0.1481087536733174</v>
       </c>
       <c r="P2" s="1">
-        <v>1.324584322994288</v>
+        <v>1.325488815396536</v>
       </c>
       <c r="Q2" s="1">
-        <v>0.3409000047751028</v>
+        <v>0.3215822963079741</v>
       </c>
       <c r="R2" s="1">
         <v>0.1838227800153526</v>
@@ -568,10 +568,10 @@
         <v>0.4667233759767803</v>
       </c>
       <c r="T2" s="1">
-        <v>0.2425652817721227</v>
+        <v>0.2425649162228197</v>
       </c>
       <c r="U2" s="1">
-        <v>0.32695342528132</v>
+        <v>0.3269535019506545</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -597,10 +597,10 @@
         <v>0.003500697815570997</v>
       </c>
       <c r="H3">
-        <v>5.1856942063239</v>
+        <v>5.185689931824315</v>
       </c>
       <c r="I3">
-        <v>0.005617505714359325</v>
+        <v>0.005759621605348021</v>
       </c>
       <c r="J3">
         <v>4.506651131411997</v>
@@ -621,22 +621,22 @@
         <v>0.0478513419537915</v>
       </c>
       <c r="P3">
-        <v>0.0032773447034385</v>
+        <v>0.003275356462361479</v>
       </c>
       <c r="Q3">
-        <v>2.118638886166868</v>
+        <v>2.119924914268915</v>
       </c>
       <c r="R3">
-        <v>0.09736895715369355</v>
+        <v>0.09733120204652208</v>
       </c>
       <c r="S3">
-        <v>0.198702951628399</v>
+        <v>0.2060866016614308</v>
       </c>
       <c r="T3">
-        <v>0.0003205476770501719</v>
+        <v>0.0003203543385384721</v>
       </c>
       <c r="U3">
-        <v>2.018904390208913</v>
+        <v>2.020137790100577</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1">
@@ -644,16 +644,16 @@
         <v>10815</v>
       </c>
       <c r="B4" s="1">
-        <v>-1.425063738750176</v>
+        <v>-1.993968138692681</v>
       </c>
       <c r="C4" s="1">
-        <v>0.001844886627987924</v>
+        <v>0.001741884743836049</v>
       </c>
       <c r="D4" s="1">
-        <v>0.01002745745125579</v>
+        <v>0.0100170998366197</v>
       </c>
       <c r="E4" s="1">
-        <v>0.8834914352253984</v>
+        <v>0.8474172615102259</v>
       </c>
       <c r="F4" s="1">
         <v>0.007140668033343761</v>
@@ -662,46 +662,46 @@
         <v>0.006578733621411427</v>
       </c>
       <c r="H4" s="1">
-        <v>2.732275900435217</v>
+        <v>2.732303424305919</v>
       </c>
       <c r="I4" s="1">
-        <v>0.01254469539256384</v>
+        <v>0.01120578579880862</v>
       </c>
       <c r="J4" s="1">
-        <v>2.071877261004955</v>
+        <v>2.073822321355093</v>
       </c>
       <c r="K4" s="1">
-        <v>0.8536139860979418</v>
+        <v>0.8201294338742942</v>
       </c>
       <c r="L4" s="1">
-        <v>0.007568340055058053</v>
+        <v>0.007564028248501297</v>
       </c>
       <c r="M4" s="1">
-        <v>0.1847519460978394</v>
+        <v>0.1745364945928616</v>
       </c>
       <c r="N4" s="1">
-        <v>5.489037688338532E-05</v>
+        <v>5.485910494195209E-05</v>
       </c>
       <c r="O4" s="1">
-        <v>0.18475194609784</v>
+        <v>0.1745364945928622</v>
       </c>
       <c r="P4" s="1">
-        <v>1.323333400550307</v>
+        <v>1.323289409733625</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.2852824024570378</v>
+        <v>0.2736660921300703</v>
       </c>
       <c r="R4" s="1">
-        <v>0.1830110572045474</v>
+        <v>0.1830152333401183</v>
       </c>
       <c r="S4" s="1">
-        <v>0.413548279079566</v>
+        <v>0.3958132555503516</v>
       </c>
       <c r="T4" s="1">
-        <v>0.2414264833758018</v>
+        <v>0.2414261194212968</v>
       </c>
       <c r="U4" s="1">
-        <v>0.3636863292778187</v>
+        <v>0.3636864051450315</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -751,10 +751,10 @@
         <v>0.04339282011123644</v>
       </c>
       <c r="P5">
-        <v>0.002813531792510626</v>
+        <v>0.002818224514931116</v>
       </c>
       <c r="Q5">
-        <v>1.997515402124657</v>
+        <v>1.876895080002627</v>
       </c>
       <c r="R5">
         <v>0.1814969380218558</v>
@@ -763,10 +763,10 @@
         <v>0.3098441651051433</v>
       </c>
       <c r="T5">
-        <v>0.0005110649611273431</v>
+        <v>0.000512323621250908</v>
       </c>
       <c r="U5">
-        <v>2.008083298503632</v>
+        <v>1.970959586851783</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="1" customFormat="1">
@@ -816,10 +816,10 @@
         <v>0.1797637951548278</v>
       </c>
       <c r="P6" s="1">
-        <v>1.322200220349557</v>
+        <v>1.32219823094449</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.2209736404250356</v>
+        <v>0.2209739728222805</v>
       </c>
       <c r="R6" s="1">
         <v>0.1811370290506207</v>
@@ -828,10 +828,10 @@
         <v>0.3803973243849685</v>
       </c>
       <c r="T6" s="1">
-        <v>0.239667028579765</v>
+        <v>0.2396666663667818</v>
       </c>
       <c r="U6" s="1">
-        <v>0.3656704039744018</v>
+        <v>0.3656704898636055</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -845,10 +845,10 @@
         <v>0.0005465452420743875</v>
       </c>
       <c r="D7">
-        <v>0.009974392941727757</v>
+        <v>0.009976845361061415</v>
       </c>
       <c r="E7">
-        <v>0.3399342746653213</v>
+        <v>0.3297874133506366</v>
       </c>
       <c r="F7">
         <v>0.007131295183894645</v>
@@ -881,10 +881,10 @@
         <v>0.04774826555039949</v>
       </c>
       <c r="P7">
-        <v>0.003654896968490784</v>
+        <v>0.003639453782854304</v>
       </c>
       <c r="Q7">
-        <v>1.936336394570503</v>
+        <v>1.822070429031099</v>
       </c>
       <c r="R7">
         <v>0.1804577480367137</v>
@@ -893,10 +893,10 @@
         <v>0.3852339957965794</v>
       </c>
       <c r="T7">
-        <v>0.0006636456736421185</v>
+        <v>0.0006632840911626782</v>
       </c>
       <c r="U7">
-        <v>1.939710498005037</v>
+        <v>1.940759177824897</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="1" customFormat="1">
@@ -946,10 +946,10 @@
         <v>0.133246697787821</v>
       </c>
       <c r="P8" s="1">
-        <v>1.319624247369094</v>
+        <v>1.319622257679337</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.2325179417830537</v>
+        <v>0.2325182917524557</v>
       </c>
       <c r="R8" s="1">
         <v>0.1803459092003151</v>
@@ -958,10 +958,10 @@
         <v>0.4297868006133961</v>
       </c>
       <c r="T8" s="1">
-        <v>0.2382822709433621</v>
+        <v>0.2382819122323587</v>
       </c>
       <c r="U8" s="1">
-        <v>0.3670470559826737</v>
+        <v>0.3670471312898169</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -969,16 +969,16 @@
         <v>10992</v>
       </c>
       <c r="B9">
-        <v>144.2738303060913</v>
+        <v>144.2477879671713</v>
       </c>
       <c r="C9">
-        <v>0.0003788097800316013</v>
+        <v>0.0003612035633638828</v>
       </c>
       <c r="D9">
-        <v>0.009984642247515869</v>
+        <v>0.00998226392451965</v>
       </c>
       <c r="E9">
-        <v>0.3249150038569073</v>
+        <v>0.3367852707192005</v>
       </c>
       <c r="F9">
         <v>0.007129198117649794</v>
@@ -993,28 +993,28 @@
         <v>0.005087385928677475</v>
       </c>
       <c r="J9">
-        <v>4.698260018102006</v>
+        <v>4.698652581306738</v>
       </c>
       <c r="K9">
-        <v>0.3272789772884239</v>
+        <v>0.3404243708834113</v>
       </c>
       <c r="L9">
-        <v>0.008672612489439223</v>
+        <v>0.008672415110885429</v>
       </c>
       <c r="M9">
-        <v>0.0331048189689242</v>
+        <v>0.03156690073271559</v>
       </c>
       <c r="N9">
-        <v>6.289925725400325E-05</v>
+        <v>6.28978257402066E-05</v>
       </c>
       <c r="O9">
-        <v>0.03310481896892375</v>
+        <v>0.03156690073271488</v>
       </c>
       <c r="P9">
-        <v>0.003181029449791472</v>
+        <v>0.003179041188988946</v>
       </c>
       <c r="Q9">
-        <v>2.136376476475425</v>
+        <v>2.1377126504212</v>
       </c>
       <c r="R9">
         <v>0.1138978916414677</v>
@@ -1023,10 +1023,10 @@
         <v>0.2496545418348033</v>
       </c>
       <c r="T9">
-        <v>0.0003632314580999754</v>
+        <v>0.0003620849407583208</v>
       </c>
       <c r="U9">
-        <v>2.136083829830561</v>
+        <v>2.044010697369161</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="1" customFormat="1">
@@ -1034,10 +1034,10 @@
         <v>10815</v>
       </c>
       <c r="B10" s="1">
-        <v>-0.7966043493090602</v>
+        <v>-1.507900421679476</v>
       </c>
       <c r="C10" s="1">
-        <v>0.001926555786283</v>
+        <v>0.001813883976860164</v>
       </c>
       <c r="D10" s="1">
         <v>0.009841760080815906</v>
@@ -1064,22 +1064,22 @@
         <v>0.9213030659910797</v>
       </c>
       <c r="L10" s="1">
-        <v>0.007573103237266384</v>
+        <v>0.007567712224173581</v>
       </c>
       <c r="M10" s="1">
-        <v>0.192809171252707</v>
+        <v>0.1816623263845749</v>
       </c>
       <c r="N10" s="1">
-        <v>5.4924922485813E-05</v>
+        <v>5.488582345771776E-05</v>
       </c>
       <c r="O10" s="1">
-        <v>0.1928091712527066</v>
+        <v>0.181662326384575</v>
       </c>
       <c r="P10" s="1">
-        <v>1.317301608640938</v>
+        <v>1.317214722714466</v>
       </c>
       <c r="Q10" s="1">
-        <v>0.2453966400949428</v>
+        <v>0.2582171694122649</v>
       </c>
       <c r="R10" s="1">
         <v>0.1802190851860907</v>
@@ -1088,10 +1088,10 @@
         <v>0.4150400840242146</v>
       </c>
       <c r="T10" s="1">
-        <v>0.2367855739726799</v>
+        <v>0.2367852110607417</v>
       </c>
       <c r="U10" s="1">
-        <v>0.4260307905930146</v>
+        <v>0.4260308980406651</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1141,22 +1141,22 @@
         <v>0.04255887954161741</v>
       </c>
       <c r="P11">
-        <v>0.003398957315546118</v>
+        <v>0.003396968616918185</v>
       </c>
       <c r="Q11">
-        <v>2.262906505247554</v>
+        <v>2.26423125468954</v>
       </c>
       <c r="R11">
-        <v>0.2062557903627206</v>
+        <v>0.2061483249746852</v>
       </c>
       <c r="S11">
-        <v>0.36315465493538</v>
+        <v>0.3523134073429333</v>
       </c>
       <c r="T11">
-        <v>0.0007053640786390493</v>
+        <v>0.0007049510064866325</v>
       </c>
       <c r="U11">
-        <v>2.296267033740035</v>
+        <v>2.297564997300947</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="1" customFormat="1">
@@ -1176,10 +1176,10 @@
         <v>0.8089106848440023</v>
       </c>
       <c r="F12" s="1">
-        <v>0.007145723959401584</v>
+        <v>0.007145697660176736</v>
       </c>
       <c r="G12" s="1">
-        <v>0.006293223271456397</v>
+        <v>0.006052072924899333</v>
       </c>
       <c r="H12" s="1">
         <v>2.731635731525279</v>
@@ -1206,10 +1206,10 @@
         <v>0.1504506050698995</v>
       </c>
       <c r="P12" s="1">
-        <v>1.316501864523344</v>
+        <v>1.317266026380881</v>
       </c>
       <c r="Q12" s="1">
-        <v>0.2613398733591065</v>
+        <v>0.245071663026405</v>
       </c>
       <c r="R12" s="1">
         <v>0.180885832906079</v>
@@ -1218,10 +1218,10 @@
         <v>0.4128124328530886</v>
       </c>
       <c r="T12" s="1">
-        <v>0.238338541222346</v>
+        <v>0.2384620925124516</v>
       </c>
       <c r="U12" s="1">
-        <v>0.4768269205556759</v>
+        <v>0.4561006561394234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>